<commit_message>
In excel removed failed data
</commit_message>
<xml_diff>
--- a/Excel/data.xlsx
+++ b/Excel/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Eclipse(Maven)\Ecommerce\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E224BED-055C-4B78-BF2A-B0647EB70FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA15EB1B-A50D-4A92-8D3F-B0F463B749DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="997">
   <si>
     <t>email</t>
   </si>
@@ -3021,12 +3021,6 @@
   </si>
   <si>
     <t>Mahaboobpasha224@gmail.com</t>
-  </si>
-  <si>
-    <t>mahaboobpasha225@gmail.com</t>
-  </si>
-  <si>
-    <t>8884722589</t>
   </si>
 </sst>
 </file>
@@ -10008,7 +10002,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10026,17 +10020,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>997</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>998</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" xr:uid="{0A750657-1893-44A8-A225-62A3663CB55D}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{945988CF-F2BC-44E5-84FB-D71671C5C029}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>